<commit_message>
updated utelies password encryption
</commit_message>
<xml_diff>
--- a/TestPracticeWebdriver/src/test/resources/testdata.xlsx
+++ b/TestPracticeWebdriver/src/test/resources/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13950" windowHeight="6075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14925" windowHeight="6075"/>
   </bookViews>
   <sheets>
     <sheet name="testing" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <t>77378</t>
   </si>
   <si>
-    <t>Cfg@2021$</t>
+    <t>Q2ZnQDIwMjEk</t>
   </si>
 </sst>
 </file>
@@ -363,7 +363,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added encoded password utility
</commit_message>
<xml_diff>
--- a/TestPracticeWebdriver/src/test/resources/testdata.xlsx
+++ b/TestPracticeWebdriver/src/test/resources/testdata.xlsx
@@ -3,11 +3,6 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shekhar\git\POMPractice\TestPracticeWebdriver\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14925" windowHeight="6075"/>
   </bookViews>
@@ -15,6 +10,7 @@
     <sheet name="testing" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +31,7 @@
     <t>77378</t>
   </si>
   <si>
-    <t>Q2ZnQDIwMjEk</t>
+    <t>config:approverpassword</t>
   </si>
 </sst>
 </file>
@@ -369,7 +365,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated dataprovider - invalid/valid sheet from same excel using TestNG method
</commit_message>
<xml_diff>
--- a/TestPracticeWebdriver/src/test/resources/testdata.xlsx
+++ b/TestPracticeWebdriver/src/test/resources/testdata.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="14925" windowHeight="6075"/>
   </bookViews>
   <sheets>
-    <sheet name="testing" sheetId="1" r:id="rId1"/>
+    <sheet name="validScenario" sheetId="1" r:id="rId1"/>
+    <sheet name="invalidScenario" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>username</t>
   </si>
@@ -36,6 +37,9 @@
   </si>
   <si>
     <t>77378</t>
+  </si>
+  <si>
+    <t>1234</t>
   </si>
 </sst>
 </file>
@@ -378,7 +382,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,4 +412,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
refactord code - 24th june
</commit_message>
<xml_diff>
--- a/TestPracticeWebdriver/src/test/resources/testdata.xlsx
+++ b/TestPracticeWebdriver/src/test/resources/testdata.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shekhar\git\POMPractice\TestPracticeWebdriver\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14925" windowHeight="6075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14925" windowHeight="6075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="validScenario" sheetId="1" r:id="rId1"/>
     <sheet name="invalidScenario" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:M18"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -381,7 +377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -418,7 +414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>